<commit_message>
digital technology and self
</commit_message>
<xml_diff>
--- a/impacts of digital technologies on people's self conceptions/Spreadsheet/annotated bibliography_technology and self image.xlsx
+++ b/impacts of digital technologies on people's self conceptions/Spreadsheet/annotated bibliography_technology and self image.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/norhantarek/Documents/GitHub/GA-Research-Dr-Misra/impacts of digital technologies on people's self conceptions/Spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9A8EF4-3EEA-CE41-9AFE-66E5A7D3FF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9B2934-3F74-E243-B807-CD873E286099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" xr2:uid="{C1520DBA-41E6-574A-ACEF-F3B95E4D5F58}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="211">
   <si>
     <t>Author</t>
   </si>
@@ -687,6 +687,174 @@
   </si>
   <si>
     <t>Adolescent girls have emerged as the largest demographic of bloggers in the United States. In this study, the author interviewed 20 girls, aged 17 to 21, who had been blogging for 3 or more years. Consistent with previous studies involving youths’ online activities, the girls discussed their use of blogging for self-expression and peer interaction. They also observed that the content and style of their blog writing has changed considerably over the years. Their observations reflect key changes in self-development and peer relationships that typically occur during the transition from adolescence to emerging adulthood. Drawing on these findings, the author presents a conceptual framework that illustrates how developmental theory can illuminate our understanding of adolescents’ and emerging adults’ online behaviors.</t>
+  </si>
+  <si>
+    <t>Predicting Self-Disclosure in Recruitment in the Context of Social Media Screening</t>
+  </si>
+  <si>
+    <t>Debora JeskeSonia LippkeKenneth S Shultz</t>
+  </si>
+  <si>
+    <t>Employee Responsibilities and Rights Journal</t>
+  </si>
+  <si>
+    <t>n2 (20190615)</t>
+  </si>
+  <si>
+    <t>v31</t>
+  </si>
+  <si>
+    <t>99-112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+10.1007/s10672-019-09329-8</t>
+  </si>
+  <si>
+    <t>https://link-springer-com.ezproxy.lib.vt.edu/content/pdf/10.1007/s10672-019-09329-8.pdf</t>
+  </si>
+  <si>
+    <t>Understanding the factors that support the self-disclosure of information by prospective job
+applicants in recruitment settings provide an important means to understand withdrawal from
+and completion of applications for job vacancies, particularly in the age of increasing social
+media screening (also known as cyber-vetting). The general willingness to trust others, the
+anticipated (mis)use of information (e.g., that may disadvantage applicants), and global
+privacy concerns may all influence applicant completion and withdrawal behaviors. The
+purpose of the current study was therefore to examine whether the relationship between
+perceived vulnerability regarding the use of information and general self-disclosure was
+mediated by one’s willingness to trust, as well as the link to the completion of applications.
+The authors collected data from an online sample of 222 student participants who were asked
+to respond to several hypothetical job scenarios suggesting social media screening. The results
+indicated that willingness to trust was an independent predictor of self-disclosure. However,
+while no support for mediation was found, a moderation effect transpired. Specifically, selfdisclosure was lowest when both vulnerability and global privacy concerns were high. Followup analysis showed that self-disclosure predicted intention to continue with the application
+process. This suggests that prospective applicants’ willingness to trust, privacy concerns, and
+perceived vulnerability associated with the use of information about applicants may be
+important predictors of self-disclosure involved in information sharing (and thus applications
+submission/completion rates) during recruitment.</t>
+  </si>
+  <si>
+    <t>The presentation of self in everyday life.</t>
+  </si>
+  <si>
+    <t>referenced in most articles</t>
+  </si>
+  <si>
+    <t>Erving Goffman 1922-1982.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The key work of one of the most influential sociologists of the twentieth century. Erving Goffman deals with human interaction in social situations using the metaphor of the stage. Role-playing is now recognized as not merely the province of the performer and the maladjusted neurotic, but as an integral and necessary function of daily living. Social techniques of self-presentation are illuminated by examples taken from detailed research and observation of social customs in many regions and a variety of occupational levels. One of the most interesting aspects of this study is its revelation of the many roles that must be assumed by everyone engaged in even the simplest life-situations. In the course of any day one may easily play a half-dozen parts: with the boss, with fellow-workers, with friends, with one's spouse, and so on. Dr. Goffman's analogy details how "acting" techniques are used in the most common everyday circumstances; it bares the mainsprings of manipulation that keep society moving.--From publisher description.
+</t>
+  </si>
+  <si>
+    <t>https://monoskop.org/images/1/19/Goffman_Erving_The_Presentation_of_Self_in_Everyday_Life.pdf</t>
+  </si>
+  <si>
+    <t>Increasing physical activity with mobile devices: a meta-analysis.</t>
+  </si>
+  <si>
+    <t>Fanning JMullen SPMcAuley E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+10.2196/jmir.2171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+From MEDLINE®/PubMed®, a database of the U.S. National Library of Medicine.</t>
+  </si>
+  <si>
+    <t>http://europepmc.org/article/MED/23171838?singleResult=true</t>
+  </si>
+  <si>
+    <t>Regular physical activity has established physical and mental health benefits; however, merely one quarter of the U.S. adult population meets national physical activity recommendations. In an effort to engage individuals who do not meet these guidelines, researchers have utilized popular emerging technologies, including mobile devices (ie, personal digital assistants [PDAs], mobile phones). This study is the first to synthesize current research focused on the use of mobile devices for increasing physical activity.
+Objective
+To conduct a meta-analysis of research utilizing mobile devices to influence physical activity behavior. The aims of this review were to: (1) examine the efficacy of mobile devices in the physical activity setting, (2) explore and discuss implementation of device features across studies, and (3) make recommendations for future intervention development.
+Methods
+We searched electronic databases (PubMed, PsychINFO, SCOPUS) and identified publications through reference lists and requests to experts in the field of mobile health. Studies were included that provided original data and aimed to influence physical activity through dissemination or collection of intervention materials with a mobile device. Data were extracted to calculate effect sizes for individual studies, as were study descriptives. A random effects meta-analysis was conducted using the Comprehensive Meta-Analysis software suite. Study quality was assessed using the quality of execution portion of the Guide to Community Preventative Services data extraction form.
+Results
+Four studies were of "good" quality and seven of "fair" quality. In total, 1351 individuals participated in 11 unique studies from which 18 effects were extracted and synthesized, yielding an overall weight mean effect size of g = 0.54 (95% CI = 0.17 to 0.91, P = .01).
+Conclusions
+Research utilizing mobile devices is gaining in popularity, and this study suggests that this platform is an effective means for influencing physical activity behavior. Our focus must be on the best possible use of these tools to measure and understand behavior. Therefore, theoretically grounded behavior change interventions that recognize and act on the potential of smartphone technology could provide investigators with an effective tool for increasing physical activity.</t>
+  </si>
+  <si>
+    <t>Wellbeing in the Making: Peoples’ Experiences with Wearable Activity Trackers</t>
+  </si>
+  <si>
+    <t>Evangelos KarapanosRúben GouveiaMarc HassenzahlJodi Forlizzi</t>
+  </si>
+  <si>
+    <t>Psychology of Well-Being : Theory, Research and Practice</t>
+  </si>
+  <si>
+    <t>n1 (201612)</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>1--17</t>
+  </si>
+  <si>
+    <t>10.1186/s13612-016-0042-6</t>
+  </si>
+  <si>
+    <t>Background: Wearable activity trackers have become a viable business opportunity.
+Nevertheless, research has raised concerns over their potentially detrimental effects
+on wellbeing. For example, a recent study found that while counting steps with a
+pedometer increased steps taken throughout the day, at the same time it decreased
+the enjoyment people derived from walking. This poses a serious threat to the incorporation of healthy routines into everyday life. Most studies aim at proving the effectiveness of activity trackers. In contrast, a wellbeing-oriented perspective calls for a deeper
+understanding of how trackers create and mediate meaningful experiences in everyday life.
+Methods: We present a study of real life experiences with three wearable activity
+trackers: Fitbit, Jawbone Up and Nike + Fuelband. Using need fulfillment as a theoretical lens, we study recent, memorable experiences submitted by 133 users of activity
+trackers.
+Results: We reveal a two-dimensional structure of users’ experience driven by the
+needs of physical thriving or relatedness. Our qualitative findings further show a
+nuanced picture of the adoption of activity trackers and their impact on wellbeing. For
+instance, while reflection about own exercising practices lost its relevance over time,
+users continued to wear the tracker to document and collect their runs. More than
+just supporting behavioral change, we find trackers to provide multiple psychological
+benefits. For instance, they enhance feelings of autonomy as people gain more control
+about their exercising regime. Others experience relatedness, when family members
+purchase a tracker for relatives and join them in their efforts towards a better, healthier
+self.
+Conclusions: The study highlights that activity trackers can be more than “tools” to
+change behavior. Through incorporation in daily life, they offer new social experiences,
+new ways of boosting our self-esteem and getting closer to our ideal selves.</t>
+  </si>
+  <si>
+    <t>https://psywb.springeropen.com/track/pdf/10.1186/s13612-016-0042-6.pdf</t>
+  </si>
+  <si>
+    <t>Walking in the wild—Using an always‐on smartphone
+application to increase physical activity</t>
+  </si>
+  <si>
+    <t>Harries TRettie REslambolchilar PStride CWalton S</t>
+  </si>
+  <si>
+    <t>conference article</t>
+  </si>
+  <si>
+    <t>120 LNCS nPART 4 (2013 09 05)</t>
+  </si>
+  <si>
+    <t>19-36</t>
+  </si>
+  <si>
+    <t>Lecture Notes in Computer Science (including subseries Lecture Notes in Artificial Intelligence and Lecture Notes in Bioinformatics)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Copyright 2021 Elsevier B.V. All rights reserved</t>
+  </si>
+  <si>
+    <t>https://link-springer-com.ezproxy.lib.vt.edu/chapter/10.1007/978-3-642-40498-6_2</t>
+  </si>
+  <si>
+    <t>10.1007/978-3-642-40498-6_2</t>
+  </si>
+  <si>
+    <t>This multidisciplinary paper reports on a large-scale field trial, designed and implemented by a group of social scientists, computer scientists and statisticians, of a new smartphone-based app for the promotion of walking in everyday life. The app, bActive, is designed for a more diverse range of users than the typical active-lifestyle app, since it requires neither additional equipment nor a great deal of commitment to exercise. As a result, it can raise awareness of walking and promote walking amongst those with only a casual or hesitant engagement with the topic. The 6-week randomised controlled trial with 22-40 year-old male participants (N=152) indicates that bActive prompted users to increase the amount of walking they did by encouraging them to value and increase walking that is incidental to normal everyday activities. Longitudinal data analysis showed that use of the app increased walking by an average of 64% but did not find any evidence to suggest that the inclusion of comparative social feedback improves the impact of such apps on male participants.</t>
   </si>
 </sst>
 </file>
@@ -781,7 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -789,6 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1144,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF47DCC6-58F9-2A40-93ED-9706ACF8B9A3}">
-  <dimension ref="A1:Z21"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,606 +1331,606 @@
     <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="10">
         <v>2014</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="10">
         <v>2019</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
     </row>
     <row r="4" spans="1:26" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="10">
         <v>2017</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26" ht="229" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="12" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
     </row>
     <row r="6" spans="1:26" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="10">
         <v>2007</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="224" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="10">
         <v>2015</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="10">
         <v>2019</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="10">
         <v>28</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9" t="s">
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="10">
         <v>2017</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="10">
         <v>2020</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="10">
         <v>33</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="10">
         <v>2015</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="149" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="10">
         <v>2019</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="212" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="10">
         <v>2020</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:26" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="10">
         <v>2018</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="10">
         <v>-201810</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="10">
         <v>2010</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>114</v>
       </c>
       <c r="F15" s="3">
         <v>30</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="18" t="s">
         <v>118</v>
       </c>
       <c r="L15" s="4" t="s">
@@ -1769,28 +1938,28 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="235" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="10">
         <v>2014</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="10" t="s">
         <v>126</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -1799,33 +1968,33 @@
       <c r="J16" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="L16" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:13" ht="201" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="10">
         <v>2010</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="10" t="s">
         <v>134</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -1834,39 +2003,39 @@
       <c r="I17" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="11" t="s">
         <v>138</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="225" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:13" ht="225" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="10">
         <v>2020</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>141</v>
       </c>
       <c r="F18" s="3">
         <v>22</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="10" t="s">
         <v>143</v>
       </c>
       <c r="J18" s="4" t="s">
@@ -1875,33 +2044,33 @@
       <c r="K18" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="L18" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="206" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:13" ht="206" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="10">
         <v>2017</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="10" t="s">
         <v>151</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -1910,36 +2079,36 @@
       <c r="J19" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="L19" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="229" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:13" ht="229" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="10">
         <v>2018</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="10" t="s">
         <v>158</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="10" t="s">
         <v>160</v>
       </c>
       <c r="I20" s="4" t="s">
@@ -1951,36 +2120,36 @@
       <c r="K20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L20" s="9" t="s">
+      <c r="L20" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:13" ht="239" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="10">
         <v>2010</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>166</v>
       </c>
       <c r="F21" s="3">
         <v>25</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="21" t="s">
         <v>169</v>
       </c>
       <c r="J21" s="4" t="s">
@@ -1989,8 +2158,177 @@
       <c r="K21" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="L21" s="10" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="258" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="10">
+        <v>2019</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="166" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1959</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="10">
+        <v>2012</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="3">
+        <v>14</v>
+      </c>
+      <c r="G24" s="3">
+        <v>6</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="10">
+        <v>2016</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="216" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2008,6 +2346,11 @@
     <hyperlink ref="K20" r:id="rId11" xr:uid="{3BDAA3B8-F0B7-2644-9B28-4F2536EAD134}"/>
     <hyperlink ref="I21" r:id="rId12" xr:uid="{D5973994-450C-CB40-92B3-CE3687E0543E}"/>
     <hyperlink ref="K21" r:id="rId13" xr:uid="{73F8D068-CAC2-2147-A192-D4BAF50A61E8}"/>
+    <hyperlink ref="K22" r:id="rId14" xr:uid="{D447B189-8222-B540-9016-E1DF76248453}"/>
+    <hyperlink ref="K23" r:id="rId15" xr:uid="{B72948EE-64F9-E140-BD83-604EBF5ECF1F}"/>
+    <hyperlink ref="K24" r:id="rId16" xr:uid="{6BA7B681-80C4-2447-B556-83243D6E2E8D}"/>
+    <hyperlink ref="K25" r:id="rId17" xr:uid="{6CCE8A1A-07D8-0943-9F02-59AB0B35EA55}"/>
+    <hyperlink ref="K26" r:id="rId18" xr:uid="{72D799F6-C9DD-384C-8014-946083F3CBD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>